<commit_message>
New file for stacked plots
</commit_message>
<xml_diff>
--- a/Output/merged_data.xlsx
+++ b/Output/merged_data.xlsx
@@ -1388,17 +1388,27 @@
       <c r="BQ2" t="n">
         <v>6</v>
       </c>
-      <c r="BR2" t="inlineStr"/>
+      <c r="BR2" t="n">
+        <v>7</v>
+      </c>
       <c r="BS2" t="inlineStr"/>
-      <c r="BT2" t="inlineStr"/>
+      <c r="BT2" t="n">
+        <v>6</v>
+      </c>
       <c r="BU2" t="inlineStr"/>
       <c r="BV2" t="inlineStr"/>
       <c r="BW2" t="inlineStr"/>
       <c r="BX2" t="inlineStr"/>
       <c r="BY2" t="inlineStr"/>
-      <c r="BZ2" t="inlineStr"/>
-      <c r="CA2" t="inlineStr"/>
-      <c r="CB2" t="inlineStr"/>
+      <c r="BZ2" t="n">
+        <v>6</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>6</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0</v>
+      </c>
       <c r="CC2" t="n">
         <v>1.423</v>
       </c>
@@ -1547,17 +1557,27 @@
       <c r="ED2" t="inlineStr"/>
       <c r="EE2" t="inlineStr"/>
       <c r="EF2" t="inlineStr"/>
-      <c r="EG2" t="inlineStr"/>
+      <c r="EG2" t="n">
+        <v>7</v>
+      </c>
       <c r="EH2" t="inlineStr"/>
-      <c r="EI2" t="inlineStr"/>
+      <c r="EI2" t="n">
+        <v>6</v>
+      </c>
       <c r="EJ2" t="inlineStr"/>
       <c r="EK2" t="inlineStr"/>
       <c r="EL2" t="inlineStr"/>
       <c r="EM2" t="inlineStr"/>
       <c r="EN2" t="inlineStr"/>
-      <c r="EO2" t="inlineStr"/>
-      <c r="EP2" t="inlineStr"/>
-      <c r="EQ2" t="inlineStr"/>
+      <c r="EO2" t="n">
+        <v>6</v>
+      </c>
+      <c r="EP2" t="n">
+        <v>7</v>
+      </c>
+      <c r="EQ2" t="n">
+        <v>0</v>
+      </c>
       <c r="ER2" t="n">
         <v>1.577</v>
       </c>
@@ -1743,17 +1763,27 @@
       <c r="BO3" t="inlineStr"/>
       <c r="BP3" t="inlineStr"/>
       <c r="BQ3" t="inlineStr"/>
-      <c r="BR3" t="inlineStr"/>
+      <c r="BR3" t="n">
+        <v>4</v>
+      </c>
       <c r="BS3" t="inlineStr"/>
-      <c r="BT3" t="inlineStr"/>
+      <c r="BT3" t="n">
+        <v>5</v>
+      </c>
       <c r="BU3" t="inlineStr"/>
       <c r="BV3" t="inlineStr"/>
       <c r="BW3" t="inlineStr"/>
       <c r="BX3" t="inlineStr"/>
       <c r="BY3" t="inlineStr"/>
-      <c r="BZ3" t="inlineStr"/>
-      <c r="CA3" t="inlineStr"/>
-      <c r="CB3" t="inlineStr"/>
+      <c r="BZ3" t="n">
+        <v>6</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>0</v>
+      </c>
       <c r="CC3" t="n">
         <v>2</v>
       </c>
@@ -1882,17 +1912,27 @@
       <c r="EF3" t="n">
         <v>7</v>
       </c>
-      <c r="EG3" t="inlineStr"/>
+      <c r="EG3" t="n">
+        <v>6</v>
+      </c>
       <c r="EH3" t="inlineStr"/>
-      <c r="EI3" t="inlineStr"/>
+      <c r="EI3" t="n">
+        <v>7</v>
+      </c>
       <c r="EJ3" t="inlineStr"/>
       <c r="EK3" t="inlineStr"/>
       <c r="EL3" t="inlineStr"/>
       <c r="EM3" t="inlineStr"/>
       <c r="EN3" t="inlineStr"/>
-      <c r="EO3" t="inlineStr"/>
-      <c r="EP3" t="inlineStr"/>
-      <c r="EQ3" t="inlineStr"/>
+      <c r="EO3" t="n">
+        <v>5</v>
+      </c>
+      <c r="EP3" t="n">
+        <v>7</v>
+      </c>
+      <c r="EQ3" t="n">
+        <v>0</v>
+      </c>
       <c r="ER3" t="n">
         <v>2.846</v>
       </c>
@@ -2084,17 +2124,27 @@
       <c r="BO4" t="inlineStr"/>
       <c r="BP4" t="inlineStr"/>
       <c r="BQ4" t="inlineStr"/>
-      <c r="BR4" t="inlineStr"/>
+      <c r="BR4" t="n">
+        <v>7</v>
+      </c>
       <c r="BS4" t="inlineStr"/>
-      <c r="BT4" t="inlineStr"/>
+      <c r="BT4" t="n">
+        <v>7</v>
+      </c>
       <c r="BU4" t="inlineStr"/>
       <c r="BV4" t="inlineStr"/>
       <c r="BW4" t="inlineStr"/>
       <c r="BX4" t="inlineStr"/>
       <c r="BY4" t="inlineStr"/>
-      <c r="BZ4" t="inlineStr"/>
-      <c r="CA4" t="inlineStr"/>
-      <c r="CB4" t="inlineStr"/>
+      <c r="BZ4" t="n">
+        <v>7</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>7</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>0</v>
+      </c>
       <c r="CC4" t="n">
         <v>1.923</v>
       </c>
@@ -2223,17 +2273,27 @@
       <c r="EF4" t="n">
         <v>7</v>
       </c>
-      <c r="EG4" t="inlineStr"/>
+      <c r="EG4" t="n">
+        <v>7</v>
+      </c>
       <c r="EH4" t="inlineStr"/>
-      <c r="EI4" t="inlineStr"/>
+      <c r="EI4" t="n">
+        <v>7</v>
+      </c>
       <c r="EJ4" t="inlineStr"/>
       <c r="EK4" t="inlineStr"/>
       <c r="EL4" t="inlineStr"/>
       <c r="EM4" t="inlineStr"/>
       <c r="EN4" t="inlineStr"/>
-      <c r="EO4" t="inlineStr"/>
-      <c r="EP4" t="inlineStr"/>
-      <c r="EQ4" t="inlineStr"/>
+      <c r="EO4" t="n">
+        <v>7</v>
+      </c>
+      <c r="EP4" t="n">
+        <v>7</v>
+      </c>
+      <c r="EQ4" t="n">
+        <v>0</v>
+      </c>
       <c r="ER4" t="n">
         <v>1.962</v>
       </c>

</xml_diff>